<commit_message>
AFDP-2727 when case file is created set to no assignee.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMILLE~1.ARM\ONEDRI~2\DOCUME~1\MobaXterm\slash\RemoteFiles\0\armdev@devvm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nebojsha.davidovikj\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>CASE_FILE</t>
-  </si>
-  <si>
-    <t>assignee, ann-acm</t>
   </si>
   <si>
     <t>Case File – Default access</t>
@@ -236,6 +233,9 @@
     ap.setParticipantLdapId(participantId);
     obj.getParticipants().add(ap);
 }</t>
+  </si>
+  <si>
+    <t>assignee, new String('')</t>
   </si>
 </sst>
 </file>
@@ -678,6 +678,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -713,6 +730,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -870,8 +904,8 @@
   </sheetPr>
   <dimension ref="A2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,14 +1008,14 @@
         <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="21" t="b">
         <v>0</v>
@@ -1051,19 +1085,19 @@
         <v>16</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -1086,10 +1120,10 @@
         <v>23</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1143,15 +1177,15 @@
       </c>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
-      <c r="G21" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>33</v>
@@ -1169,7 +1203,7 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>25</v>
@@ -1178,39 +1212,39 @@
         <v>26</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="19" t="s">
         <v>40</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>41</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>30</v>
@@ -1225,7 +1259,7 @@
     <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>33</v>
@@ -1235,7 +1269,7 @@
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
       <c r="H26" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1264,10 +1298,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1275,30 +1309,30 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
         <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding creator read access for new complaint
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nebojsha.davidovikj\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teng.wang\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="535"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t>RuleSet</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>assignee, new String('')</t>
+  </si>
+  <si>
+    <t>Complaint - creator read access</t>
   </si>
 </sst>
 </file>
@@ -902,26 +905,26 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:H26"/>
+  <dimension ref="A2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5546875"/>
-    <col min="2" max="2" width="24.33203125"/>
-    <col min="3" max="3" width="49.88671875"/>
-    <col min="4" max="4" width="81.77734375" customWidth="1"/>
-    <col min="5" max="5" width="43.88671875"/>
-    <col min="6" max="6" width="30.5546875"/>
-    <col min="7" max="7" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="21.54296875"/>
+    <col min="2" max="2" width="24.36328125"/>
+    <col min="3" max="3" width="49.90625"/>
+    <col min="4" max="4" width="81.81640625" customWidth="1"/>
+    <col min="5" max="5" width="43.90625"/>
+    <col min="6" max="6" width="30.54296875"/>
+    <col min="7" max="7" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.6328125"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -931,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -941,7 +944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -951,7 +954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -961,7 +964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -971,7 +974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -981,7 +984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -991,7 +994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1001,7 +1004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1011,7 +1014,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
@@ -1021,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="7" t="s">
@@ -1031,8 +1034,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
@@ -1044,7 +1047,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1066,7 +1069,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1078,7 +1081,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="10" t="s">
@@ -1100,7 +1103,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>18</v>
       </c>
@@ -1126,7 +1129,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="17" t="s">
         <v>24</v>
@@ -1146,7 +1149,7 @@
       </c>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="17" t="s">
         <v>29</v>
@@ -1164,7 +1167,7 @@
       </c>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
         <v>32</v>
@@ -1182,7 +1185,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>34</v>
@@ -1200,7 +1203,7 @@
       </c>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>35</v>
@@ -1220,7 +1223,7 @@
       </c>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>38</v>
@@ -1238,7 +1241,7 @@
       </c>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>39</v>
@@ -1256,7 +1259,7 @@
       </c>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>49</v>
@@ -1269,6 +1272,22 @@
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
       <c r="H26" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1289,14 +1308,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.6640625"/>
-    <col min="2" max="2" width="17.5546875"/>
-    <col min="3" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="18.6328125"/>
+    <col min="2" max="2" width="17.54296875"/>
+    <col min="3" max="1025" width="8.6328125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1304,7 +1323,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1312,7 +1331,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1320,17 +1339,17 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1350,9 +1369,9 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1025" width="8.6640625"/>
+    <col min="1" max="1025" width="8.6328125"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Updated the assignement rules.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nebojsha.davidovikj\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -232,10 +232,10 @@
 }</t>
   </si>
   <si>
-    <t>assignee, new String('')</t>
-  </si>
-  <si>
     <t>Complaint - creator read access</t>
+  </si>
+  <si>
+    <t>assignee, new String('ann-acm')</t>
   </si>
 </sst>
 </file>
@@ -904,24 +904,24 @@
   </sheetPr>
   <dimension ref="A2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.5703125"/>
-    <col min="2" max="2" width="24.42578125"/>
-    <col min="3" max="3" width="49.85546875"/>
-    <col min="4" max="4" width="81.85546875" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875"/>
-    <col min="6" max="6" width="30.5703125"/>
-    <col min="7" max="7" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="21.59765625"/>
+    <col min="2" max="2" width="24.3984375"/>
+    <col min="3" max="3" width="49.86328125"/>
+    <col min="4" max="4" width="81.86328125" customWidth="1"/>
+    <col min="5" max="5" width="43.86328125"/>
+    <col min="6" max="6" width="30.59765625"/>
+    <col min="7" max="7" width="42.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.59765625"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -931,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -941,7 +941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -951,7 +951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -961,7 +961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -971,7 +971,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -981,7 +981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -991,7 +991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1001,7 +1001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1011,7 +1011,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="7" t="s">
@@ -1031,8 +1031,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
@@ -1044,7 +1044,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1066,7 +1066,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1078,7 +1078,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="10" t="s">
@@ -1100,7 +1100,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
         <v>18</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="17" t="s">
         <v>24</v>
@@ -1143,10 +1143,10 @@
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
       <c r="H19" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="17" t="s">
         <v>28</v>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
         <v>31</v>
@@ -1179,10 +1179,10 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>33</v>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>34</v>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>37</v>
@@ -1238,7 +1238,7 @@
       </c>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>38</v>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>48</v>
@@ -1272,10 +1272,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>25</v>
@@ -1305,14 +1305,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.5703125"/>
-    <col min="2" max="2" width="17.5703125"/>
-    <col min="3" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="18.59765625"/>
+    <col min="2" max="2" width="17.59765625"/>
+    <col min="3" max="1025" width="8.59765625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1336,17 +1336,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1366,9 +1366,9 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1025" width="8.59765625"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
ARKCORR-18: Adding empty assignee when object is created
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riste.tutureski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -235,7 +235,7 @@
     <t>Complaint - creator read access</t>
   </si>
   <si>
-    <t>assignee, new String('ann-acm')</t>
+    <t>assignee, new String('')</t>
   </si>
 </sst>
 </file>
@@ -905,23 +905,23 @@
   <dimension ref="A2:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.59765625"/>
-    <col min="2" max="2" width="24.3984375"/>
-    <col min="3" max="3" width="49.86328125"/>
-    <col min="4" max="4" width="81.86328125" customWidth="1"/>
-    <col min="5" max="5" width="43.86328125"/>
-    <col min="6" max="6" width="30.59765625"/>
-    <col min="7" max="7" width="42.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.59765625"/>
+    <col min="1" max="1" width="21.5703125"/>
+    <col min="2" max="2" width="24.42578125"/>
+    <col min="3" max="3" width="49.85546875"/>
+    <col min="4" max="4" width="81.85546875" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875"/>
+    <col min="6" max="6" width="30.5703125"/>
+    <col min="7" max="7" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -931,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -941,7 +941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -951,7 +951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -961,7 +961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -971,7 +971,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -981,7 +981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -991,7 +991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1001,7 +1001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1011,7 +1011,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="7" t="s">
@@ -1031,8 +1031,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
@@ -1044,7 +1044,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1066,7 +1066,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1078,7 +1078,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="10" t="s">
@@ -1100,7 +1100,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>18</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="17" t="s">
         <v>24</v>
@@ -1146,7 +1146,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="17" t="s">
         <v>28</v>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
         <v>31</v>
@@ -1182,7 +1182,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>33</v>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>34</v>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>37</v>
@@ -1238,7 +1238,7 @@
       </c>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>38</v>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>48</v>
@@ -1272,7 +1272,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>56</v>
@@ -1305,14 +1305,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.59765625"/>
-    <col min="2" max="2" width="17.59765625"/>
-    <col min="3" max="1025" width="8.59765625"/>
+    <col min="1" max="1" width="18.5703125"/>
+    <col min="2" max="2" width="17.5703125"/>
+    <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1336,17 +1336,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1366,9 +1366,9 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.59765625"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
ARKCORR-30: Show Suspend queue
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8205" tabRatio="535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8210" tabRatio="535"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
     <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t>RuleSet</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>assignee, new String('')</t>
+  </si>
+  <si>
+    <t>assignee, new String('ann-acm')</t>
   </si>
 </sst>
 </file>
@@ -905,23 +908,23 @@
   <dimension ref="A2:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5703125"/>
-    <col min="2" max="2" width="24.42578125"/>
-    <col min="3" max="3" width="49.85546875"/>
-    <col min="4" max="4" width="81.85546875" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875"/>
-    <col min="6" max="6" width="30.5703125"/>
-    <col min="7" max="7" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="21.54296875"/>
+    <col min="2" max="2" width="24.453125"/>
+    <col min="3" max="3" width="49.81640625"/>
+    <col min="4" max="4" width="81.81640625" customWidth="1"/>
+    <col min="5" max="5" width="43.81640625"/>
+    <col min="6" max="6" width="30.54296875"/>
+    <col min="7" max="7" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -931,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -941,7 +944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -951,7 +954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -961,7 +964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -971,7 +974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -981,7 +984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -991,7 +994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1001,7 +1004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1011,7 +1014,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
@@ -1021,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="7" t="s">
@@ -1031,8 +1034,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
@@ -1044,7 +1047,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1066,7 +1069,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1078,7 +1081,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="10" t="s">
@@ -1100,7 +1103,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>18</v>
       </c>
@@ -1126,7 +1129,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="17" t="s">
         <v>24</v>
@@ -1146,7 +1149,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="17" t="s">
         <v>28</v>
@@ -1164,7 +1167,7 @@
       </c>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
         <v>31</v>
@@ -1179,10 +1182,10 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>33</v>
@@ -1200,7 +1203,7 @@
       </c>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>34</v>
@@ -1220,7 +1223,7 @@
       </c>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>37</v>
@@ -1238,7 +1241,7 @@
       </c>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>38</v>
@@ -1256,7 +1259,7 @@
       </c>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>48</v>
@@ -1272,7 +1275,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>56</v>
@@ -1305,14 +1308,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125"/>
-    <col min="2" max="2" width="17.5703125"/>
-    <col min="3" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="18.54296875"/>
+    <col min="2" max="2" width="17.54296875"/>
+    <col min="3" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1328,7 +1331,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1336,17 +1339,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1366,9 +1369,9 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1025" width="8.54296875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Removing added assignee by mistake
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>RuleSet</t>
   </si>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t>assignee, new String('')</t>
-  </si>
-  <si>
-    <t>assignee, new String('ann-acm')</t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1179,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Revert to  git commit 46b88bb7bb529ae4823e4cea9f48a3eb2b299fe3
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riste.tutureski\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nebojsha.davidovikj\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8210" tabRatio="535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8205" tabRatio="535"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
     <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -232,10 +232,10 @@
 }</t>
   </si>
   <si>
+    <t>assignee, new String('')</t>
+  </si>
+  <si>
     <t>Complaint - creator read access</t>
-  </si>
-  <si>
-    <t>assignee, new String('')</t>
   </si>
 </sst>
 </file>
@@ -904,24 +904,24 @@
   </sheetPr>
   <dimension ref="A2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875"/>
-    <col min="2" max="2" width="24.453125"/>
-    <col min="3" max="3" width="49.81640625"/>
-    <col min="4" max="4" width="81.81640625" customWidth="1"/>
-    <col min="5" max="5" width="43.81640625"/>
-    <col min="6" max="6" width="30.54296875"/>
-    <col min="7" max="7" width="42.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.54296875"/>
+    <col min="1" max="1" width="21.5703125"/>
+    <col min="2" max="2" width="24.42578125"/>
+    <col min="3" max="3" width="49.85546875"/>
+    <col min="4" max="4" width="81.85546875" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875"/>
+    <col min="6" max="6" width="30.5703125"/>
+    <col min="7" max="7" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -931,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -941,7 +941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -951,7 +951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -961,7 +961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -971,7 +971,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -981,7 +981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -991,7 +991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1001,7 +1001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1011,7 +1011,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="7" t="s">
@@ -1031,8 +1031,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
@@ -1044,7 +1044,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1066,7 +1066,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1078,7 +1078,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="10" t="s">
@@ -1100,7 +1100,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>18</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="17" t="s">
         <v>24</v>
@@ -1143,10 +1143,10 @@
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
       <c r="H19" s="19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="17" t="s">
         <v>28</v>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
         <v>31</v>
@@ -1179,10 +1179,10 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>33</v>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>34</v>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>37</v>
@@ -1238,7 +1238,7 @@
       </c>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>38</v>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>48</v>
@@ -1272,10 +1272,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>25</v>
@@ -1305,14 +1305,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875"/>
-    <col min="2" max="2" width="17.54296875"/>
-    <col min="3" max="1025" width="8.54296875"/>
+    <col min="1" max="1" width="18.5703125"/>
+    <col min="2" max="2" width="17.5703125"/>
+    <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1336,17 +1336,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1366,9 +1366,9 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.54296875"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Revert to  git commit 87b6f05e1224562ec5b3bce865f80a88ad93596e
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riste.tutureski\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nebojsha.davidovikj\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8210" tabRatio="535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8205" tabRatio="535"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
     <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -232,10 +232,10 @@
 }</t>
   </si>
   <si>
+    <t>assignee, new String('')</t>
+  </si>
+  <si>
     <t>Complaint - creator read access</t>
-  </si>
-  <si>
-    <t>assignee, new String('')</t>
   </si>
 </sst>
 </file>
@@ -904,24 +904,24 @@
   </sheetPr>
   <dimension ref="A2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875"/>
-    <col min="2" max="2" width="24.453125"/>
-    <col min="3" max="3" width="49.81640625"/>
-    <col min="4" max="4" width="81.81640625" customWidth="1"/>
-    <col min="5" max="5" width="43.81640625"/>
-    <col min="6" max="6" width="30.54296875"/>
-    <col min="7" max="7" width="42.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.54296875"/>
+    <col min="1" max="1" width="21.5703125"/>
+    <col min="2" max="2" width="24.42578125"/>
+    <col min="3" max="3" width="49.85546875"/>
+    <col min="4" max="4" width="81.85546875" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875"/>
+    <col min="6" max="6" width="30.5703125"/>
+    <col min="7" max="7" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -931,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -941,7 +941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -951,7 +951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -961,7 +961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -971,7 +971,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -981,7 +981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -991,7 +991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1001,7 +1001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1011,7 +1011,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="7" t="s">
@@ -1031,8 +1031,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
@@ -1044,7 +1044,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1066,7 +1066,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1078,7 +1078,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="10" t="s">
@@ -1100,7 +1100,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>18</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="17" t="s">
         <v>24</v>
@@ -1143,10 +1143,10 @@
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
       <c r="H19" s="19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="17" t="s">
         <v>28</v>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
         <v>31</v>
@@ -1179,10 +1179,10 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>33</v>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>34</v>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>37</v>
@@ -1238,7 +1238,7 @@
       </c>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>38</v>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>48</v>
@@ -1272,10 +1272,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>25</v>
@@ -1305,14 +1305,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875"/>
-    <col min="2" max="2" width="17.54296875"/>
-    <col min="3" max="1025" width="8.54296875"/>
+    <col min="1" max="1" width="18.5703125"/>
+    <col min="2" max="2" width="17.5703125"/>
+    <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1336,17 +1336,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1366,9 +1366,9 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.54296875"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Fixing addParticipant method in assignment rules
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadica.cuculova\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riste.tutureski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -195,6 +195,30 @@
     <t>Assign a participant.  First value must be the participant type, second value must be an SpEL expression that is valid when evaluated against the $acmObject.</t>
   </si>
   <si>
+    <t>assignee, new String('')</t>
+  </si>
+  <si>
+    <t>Complaint - creator read access</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Default access</t>
+  </si>
+  <si>
+    <t>DOC_REPO</t>
+  </si>
+  <si>
+    <t>DocumentRepository – Default assignee</t>
+  </si>
+  <si>
+    <t>repositoryType == 'PERSONAL'</t>
+  </si>
+  <si>
+    <t>assignee, creator</t>
+  </si>
+  <si>
+    <t>creator != null</t>
+  </si>
+  <si>
     <t>function Boolean evalBoolean(String expression, Object obj)
 {
     ExpressionParser ep = new SpelExpressionParser();
@@ -209,51 +233,22 @@
     Expression exp = ep.parseExpression(expression);
     EvaluationContext ec = new StandardEvaluationContext();
     String evaluated = exp.getValue(ec, obj, String.class);
-    boolean found = false;
-    for ( AcmParticipant ap : obj.getParticipants() )
-    {
-       if ( ap.getParticipantLdapId().equals(evaluated) &amp;&amp; ap.getParticipantType().equals(participantType) )
-      {
-        found = true;
-        break;
-      }
-    }
-    if (!found) 
-    {
-     addParticipant(obj, participantType, evaluated);
-    }
+    addParticipant(obj, participantType, evaluated);
 }
 function void addParticipant(AcmAssignedObject obj, String participantType, String participantId)
 {
+    for ( AcmParticipant ap : obj.getParticipants() )
+    {
+       if ( ap.getParticipantLdapId().equals(participantId) &amp;&amp; ap.getParticipantType().equals(participantType) )
+      {
+        return;
+      }
+    }
     AcmParticipant ap = new AcmParticipant();
     ap.setParticipantType(participantType);
     ap.setParticipantLdapId(participantId);
     obj.getParticipants().add(ap);
 }</t>
-  </si>
-  <si>
-    <t>assignee, new String('')</t>
-  </si>
-  <si>
-    <t>Complaint - creator read access</t>
-  </si>
-  <si>
-    <t>DocumentRepository – Default access</t>
-  </si>
-  <si>
-    <t>DOC_REPO</t>
-  </si>
-  <si>
-    <t>DocumentRepository – Default assignee</t>
-  </si>
-  <si>
-    <t>repositoryType == 'PERSONAL'</t>
-  </si>
-  <si>
-    <t>assignee, creator</t>
-  </si>
-  <si>
-    <t>creator != null</t>
   </si>
 </sst>
 </file>
@@ -922,8 +917,8 @@
   </sheetPr>
   <dimension ref="A2:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1021,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1161,7 +1156,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
       <c r="H19" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1197,7 +1192,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1293,7 +1288,7 @@
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>25</v>
@@ -1308,10 +1303,10 @@
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>58</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>59</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>29</v>
@@ -1325,21 +1320,21 @@
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="19" t="s">
         <v>60</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>61</v>
       </c>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
       <c r="H29" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AFDP-4502: Append domain to user/group ids in config files
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bojan.milenkoski\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadica.cuculova\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>participants.?[participantType == 'owning group'].isEmpty()</t>
-  </si>
-  <si>
-    <t>owning group, ACM_INVESTIGATOR_DEV</t>
   </si>
   <si>
     <t>Case File – Default group</t>
@@ -266,9 +263,6 @@
     <t>Organization – Default owner</t>
   </si>
   <si>
-    <t>owning group, ACM_ADMINISTRATOR_DEV</t>
-  </si>
-  <si>
     <t>owner, creator</t>
   </si>
   <si>
@@ -282,6 +276,12 @@
   </si>
   <si>
     <t>Person – Default group</t>
+  </si>
+  <si>
+    <t>owning group, ACM_INVESTIGATOR_DEV@ARMEDIA.COM</t>
+  </si>
+  <si>
+    <t>owning group, ACM_ADMINISTRATOR_DEV@ARMEDIA.COM</t>
   </si>
 </sst>
 </file>
@@ -950,8 +950,8 @@
   </sheetPr>
   <dimension ref="A2:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,7 +962,7 @@
     <col min="4" max="4" width="81.85546875" customWidth="1"/>
     <col min="5" max="5" width="43.85546875"/>
     <col min="6" max="6" width="30.5703125"/>
-    <col min="7" max="7" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.7109375" customWidth="1"/>
     <col min="8" max="8" width="62.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="1025" width="8.5703125"/>
   </cols>
@@ -1054,14 +1054,14 @@
         <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="21" t="b">
         <v>0</v>
@@ -1131,19 +1131,19 @@
         <v>16</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -1166,10 +1166,10 @@
         <v>23</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1189,7 +1189,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
       <c r="H19" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1225,7 +1225,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
       <c r="H21" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1262,14 +1262,14 @@
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>32</v>
@@ -1280,17 +1280,17 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="19" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="19" t="s">
         <v>38</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>39</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>29</v>
@@ -1305,7 +1305,7 @@
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>32</v>
@@ -1315,13 +1315,13 @@
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
       <c r="H26" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>25</v>
@@ -1331,15 +1331,15 @@
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
       <c r="H27" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>57</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>58</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>29</v>
@@ -1353,29 +1353,29 @@
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="19" t="s">
         <v>59</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>60</v>
       </c>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
       <c r="H29" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="20" t="s">
         <v>64</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>65</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>29</v>
@@ -1389,29 +1389,29 @@
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
       <c r="H31" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>35</v>
@@ -1419,16 +1419,16 @@
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="H32" s="19"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D33" s="18" t="s">
         <v>29</v>
@@ -1442,29 +1442,29 @@
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
       <c r="H34" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>35</v>
@@ -1472,7 +1472,7 @@
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
       <c r="G35" s="19" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="H35" s="19"/>
     </row>
@@ -1502,10 +1502,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1513,30 +1513,30 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
         <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Entity Administrator role reverted
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -279,10 +279,10 @@
     <t>DocumentRepository – Default group</t>
   </si>
   <si>
-    <t>owning group, ENTITY_ADMINISTRATOR_DEV@ARMEDIA.COM</t>
-  </si>
-  <si>
     <t>DocumentRepository – Default owner</t>
+  </si>
+  <si>
+    <t>owning group, ACM_ADMINISTRATOR_DEV@ARMEDIA.COM</t>
   </si>
 </sst>
 </file>
@@ -951,8 +951,8 @@
   </sheetPr>
   <dimension ref="A2:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,13 +1383,13 @@
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H30" s="19"/>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31" s="19" t="s">
         <v>57</v>
@@ -1455,7 +1455,7 @@
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
       <c r="G34" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H34" s="19"/>
     </row>
@@ -1508,7 +1508,7 @@
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
       <c r="G37" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H37" s="19"/>
     </row>

</xml_diff>

<commit_message>
AFDP-6132 fix user/groups names with correct prefix and domain
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivana.shekerova\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nebojsha\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E566C3-1E42-4000-9E7E-A54DAD508C50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9541AA0C-E64A-4FEA-A5ED-C394E6160370}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
     <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -200,9 +200,6 @@
     <t>participants.?[participantType == 'owning group'].isEmpty()</t>
   </si>
   <si>
-    <t>owning group, ARKCASE_SUPERVISOR@ARMEDIA.COM</t>
-  </si>
-  <si>
     <t>Case File – Default group</t>
   </si>
   <si>
@@ -266,9 +263,6 @@
     <t>Organization – Default group</t>
   </si>
   <si>
-    <t>owning group, ARKCASE_ENTITY_ADMINISTRATOR@ARMEDIA.COM</t>
-  </si>
-  <si>
     <t>Person – Default access</t>
   </si>
   <si>
@@ -312,6 +306,12 @@
   </si>
   <si>
     <t>Costsheet - creator read access</t>
+  </si>
+  <si>
+    <t>owning group, 000.ARKCASE_ENTITY_ADMINISTRATOR@APPDEV.ARMEDIA.COM</t>
+  </si>
+  <si>
+    <t>owning group, 000.ARKCASE_SUPERVISOR@APPDEV.ARMEDIA.COM</t>
   </si>
 </sst>
 </file>
@@ -979,24 +979,24 @@
   </sheetPr>
   <dimension ref="A2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" customWidth="1"/>
-    <col min="3" max="3" width="49.81640625" customWidth="1"/>
-    <col min="4" max="4" width="81.81640625" customWidth="1"/>
-    <col min="5" max="5" width="43.81640625" customWidth="1"/>
-    <col min="6" max="6" width="30.54296875" customWidth="1"/>
-    <col min="7" max="7" width="42.453125" customWidth="1"/>
-    <col min="8" max="8" width="62.54296875" customWidth="1"/>
-    <col min="9" max="1025" width="8.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.85546875" customWidth="1"/>
+    <col min="4" max="4" width="81.85546875" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="42.42578125" customWidth="1"/>
+    <col min="8" max="8" width="62.5703125" customWidth="1"/>
+    <col min="9" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -1006,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -1016,7 +1016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -1026,7 +1026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -1036,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -1046,7 +1046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1056,7 +1056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1066,7 +1066,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1076,7 +1076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1086,7 +1086,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
@@ -1097,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="7" t="s">
@@ -1108,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
@@ -1120,7 +1120,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1142,7 +1142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1154,7 +1154,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="10" t="s">
@@ -1176,7 +1176,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>22</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="17" t="s">
         <v>30</v>
@@ -1222,7 +1222,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="17" t="s">
         <v>35</v>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
         <v>38</v>
@@ -1258,7 +1258,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>40</v>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>41</v>
@@ -1292,14 +1292,14 @@
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>39</v>
@@ -1310,17 +1310,17 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="19" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="19" t="s">
         <v>45</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>46</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>36</v>
@@ -1332,13 +1332,13 @@
       </c>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>36</v>
@@ -1350,10 +1350,10 @@
       </c>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>39</v>
@@ -1363,13 +1363,13 @@
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
       <c r="H27" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" s="19" t="s">
         <v>31</v>
@@ -1379,18 +1379,18 @@
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
       <c r="H28" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="D29" s="18" t="s">
         <v>53</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>54</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
@@ -1399,48 +1399,48 @@
       </c>
       <c r="H29" s="19"/>
     </row>
-    <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="19" t="s">
         <v>55</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>56</v>
       </c>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="H30" s="19"/>
     </row>
-    <row r="31" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="18" t="s">
+      <c r="E31" s="19" t="s">
         <v>58</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>59</v>
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
       <c r="H31" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="17" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="B32" s="17" t="s">
+      <c r="C32" s="20" t="s">
         <v>61</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>62</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>36</v>
@@ -1452,31 +1452,31 @@
       </c>
       <c r="H32" s="19"/>
     </row>
-    <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="19" t="s">
         <v>58</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>59</v>
       </c>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
       <c r="H33" s="19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>42</v>
@@ -1484,16 +1484,16 @@
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
       <c r="G34" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="H34" s="19"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="20" t="s">
         <v>65</v>
-      </c>
-      <c r="H34" s="19"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B35" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>67</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>36</v>
@@ -1505,31 +1505,31 @@
       </c>
       <c r="H35" s="19"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D36" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="19" t="s">
         <v>58</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>59</v>
       </c>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
       <c r="H36" s="19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>42</v>
@@ -1537,16 +1537,16 @@
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
       <c r="G37" s="19" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="H37" s="19"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>36</v>
@@ -1558,41 +1558,41 @@
       </c>
       <c r="H38" s="19"/>
     </row>
-    <row r="39" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
       <c r="H39" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D40" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="19" t="s">
         <v>58</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>59</v>
       </c>
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
       <c r="H40" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1612,50 +1612,50 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" customWidth="1"/>
-    <col min="3" max="1025" width="8.54296875" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>73</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1673,9 +1673,9 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.54296875" customWidth="1"/>
+    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Updated default owning group in drools
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nebojsha\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivana.shekerova\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9541AA0C-E64A-4FEA-A5ED-C394E6160370}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E566C3-1E42-4000-9E7E-A54DAD508C50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
     <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="179021" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -200,6 +200,9 @@
     <t>participants.?[participantType == 'owning group'].isEmpty()</t>
   </si>
   <si>
+    <t>owning group, ARKCASE_SUPERVISOR@ARMEDIA.COM</t>
+  </si>
+  <si>
     <t>Case File – Default group</t>
   </si>
   <si>
@@ -263,6 +266,9 @@
     <t>Organization – Default group</t>
   </si>
   <si>
+    <t>owning group, ARKCASE_ENTITY_ADMINISTRATOR@ARMEDIA.COM</t>
+  </si>
+  <si>
     <t>Person – Default access</t>
   </si>
   <si>
@@ -306,12 +312,6 @@
   </si>
   <si>
     <t>Costsheet - creator read access</t>
-  </si>
-  <si>
-    <t>owning group, 000.ARKCASE_ENTITY_ADMINISTRATOR@APPDEV.ARMEDIA.COM</t>
-  </si>
-  <si>
-    <t>owning group, 000.ARKCASE_SUPERVISOR@APPDEV.ARMEDIA.COM</t>
   </si>
 </sst>
 </file>
@@ -979,24 +979,24 @@
   </sheetPr>
   <dimension ref="A2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="C30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49.85546875" customWidth="1"/>
-    <col min="4" max="4" width="81.85546875" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" customWidth="1"/>
-    <col min="8" max="8" width="62.5703125" customWidth="1"/>
-    <col min="9" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="49.81640625" customWidth="1"/>
+    <col min="4" max="4" width="81.81640625" customWidth="1"/>
+    <col min="5" max="5" width="43.81640625" customWidth="1"/>
+    <col min="6" max="6" width="30.54296875" customWidth="1"/>
+    <col min="7" max="7" width="42.453125" customWidth="1"/>
+    <col min="8" max="8" width="62.54296875" customWidth="1"/>
+    <col min="9" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -1006,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -1016,7 +1016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -1026,7 +1026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -1036,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -1046,7 +1046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1056,7 +1056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1066,7 +1066,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1076,7 +1076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1086,7 +1086,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
@@ -1097,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="7" t="s">
@@ -1108,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
@@ -1120,7 +1120,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1142,7 +1142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1154,7 +1154,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="10" t="s">
@@ -1176,7 +1176,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>22</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="17" t="s">
         <v>30</v>
@@ -1222,7 +1222,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="17" t="s">
         <v>35</v>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
         <v>38</v>
@@ -1258,7 +1258,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>40</v>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>41</v>
@@ -1292,14 +1292,14 @@
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>39</v>
@@ -1310,17 +1310,17 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="19" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>36</v>
@@ -1332,13 +1332,13 @@
       </c>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>36</v>
@@ -1350,10 +1350,10 @@
       </c>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>39</v>
@@ -1363,13 +1363,13 @@
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
       <c r="H27" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C28" s="19" t="s">
         <v>31</v>
@@ -1379,18 +1379,18 @@
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
       <c r="H28" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="B29" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
@@ -1399,48 +1399,48 @@
       </c>
       <c r="H29" s="19"/>
     </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="B30" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="H30" s="19"/>
     </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="B31" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
       <c r="H31" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="B32" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>36</v>
@@ -1452,31 +1452,31 @@
       </c>
       <c r="H32" s="19"/>
     </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="B33" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="20" t="s">
-        <v>61</v>
-      </c>
       <c r="D33" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
       <c r="H33" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="B34" s="17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>42</v>
@@ -1484,16 +1484,16 @@
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
       <c r="G34" s="19" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="H34" s="19"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B35" s="17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>36</v>
@@ -1505,31 +1505,31 @@
       </c>
       <c r="H35" s="19"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B36" s="17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
       <c r="H36" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B37" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="20" t="s">
         <v>67</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>65</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>42</v>
@@ -1537,16 +1537,16 @@
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
       <c r="G37" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H37" s="19"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="H37" s="19"/>
-    </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="17" t="s">
-        <v>77</v>
-      </c>
       <c r="C38" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>36</v>
@@ -1558,41 +1558,41 @@
       </c>
       <c r="H38" s="19"/>
     </row>
-    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="19" t="s">
         <v>78</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>76</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
       <c r="H39" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B40" s="17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
       <c r="H40" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1612,50 +1612,50 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
+    <col min="3" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1673,9 +1673,9 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
AFDP-8987 Consultation Configuration Update Init
- Add access control rules for the new consultation module
- Add new consultation module, list, save, create privileges
- Add new default consultation Alfresco paths
- Add initial assignment rules for consultations
- Add new consultation rules
</commit_message>
<xml_diff>
--- a/acm/rules/drools-assignment-rules.xlsx
+++ b/acm/rules/drools-assignment-rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivana.shekerova\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleksandar.acevski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06871977-1957-4925-983C-7F8F63F0034F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1793F7E3-7BB9-47AE-A9CC-497FF0A5C0F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
     <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="86">
   <si>
     <t>RuleSet</t>
   </si>
@@ -314,6 +314,21 @@
   <si>
     <t>ACCESS CONTROL LIST</t>
   </si>
+  <si>
+    <t>Consultation - creator read access</t>
+  </si>
+  <si>
+    <t>Consultation – Default assignee</t>
+  </si>
+  <si>
+    <t>Consultation – Default access</t>
+  </si>
+  <si>
+    <t>Consultation – Default group</t>
+  </si>
+  <si>
+    <t>CONSULTATION</t>
+  </si>
 </sst>
 </file>
 
@@ -322,7 +337,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -989,26 +1004,26 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A2:H40"/>
+  <dimension ref="A2:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49.85546875" customWidth="1"/>
-    <col min="4" max="4" width="81.85546875" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" customWidth="1"/>
-    <col min="8" max="8" width="62.5703125" customWidth="1"/>
-    <col min="9" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.59765625" customWidth="1"/>
+    <col min="2" max="2" width="24.3984375" customWidth="1"/>
+    <col min="3" max="3" width="49.86328125" customWidth="1"/>
+    <col min="4" max="4" width="81.86328125" customWidth="1"/>
+    <col min="5" max="5" width="43.86328125" customWidth="1"/>
+    <col min="6" max="6" width="30.59765625" customWidth="1"/>
+    <col min="7" max="7" width="46.73046875" customWidth="1"/>
+    <col min="8" max="8" width="62.59765625" customWidth="1"/>
+    <col min="9" max="1025" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -1018,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -1028,7 +1043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -1038,7 +1053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -1048,7 +1063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -1058,7 +1073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1068,7 +1083,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1078,7 +1093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1088,7 +1103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1098,7 +1113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="7" t="s">
@@ -1109,7 +1124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="7" t="s">
@@ -1120,7 +1135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
@@ -1132,7 +1147,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1154,7 +1169,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1166,7 +1181,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="10" t="s">
@@ -1188,7 +1203,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="87">
+    <row r="18" spans="1:8" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
         <v>22</v>
       </c>
@@ -1214,7 +1229,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="29.1">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="17" t="s">
         <v>30</v>
@@ -1234,7 +1249,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="17" t="s">
         <v>35</v>
@@ -1252,7 +1267,7 @@
       </c>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
         <v>38</v>
@@ -1270,7 +1285,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>40</v>
@@ -1288,7 +1303,7 @@
       </c>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" ht="30">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>41</v>
@@ -1308,7 +1323,7 @@
       </c>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="1:8" ht="15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>44</v>
@@ -1326,7 +1341,7 @@
       </c>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>45</v>
@@ -1344,7 +1359,7 @@
       </c>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>47</v>
@@ -1362,7 +1377,7 @@
       </c>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="1:8" ht="29.1">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>49</v>
@@ -1378,7 +1393,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="29.1">
+    <row r="28" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
         <v>51</v>
@@ -1394,7 +1409,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="29.1">
+    <row r="29" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B29" s="17" t="s">
         <v>52</v>
       </c>
@@ -1411,7 +1426,7 @@
       </c>
       <c r="H29" s="19"/>
     </row>
-    <row r="30" spans="1:8" ht="30">
+    <row r="30" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B30" s="17" t="s">
         <v>55</v>
       </c>
@@ -1428,7 +1443,7 @@
       </c>
       <c r="H30" s="19"/>
     </row>
-    <row r="31" spans="1:8" ht="29.1">
+    <row r="31" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B31" s="17" t="s">
         <v>57</v>
       </c>
@@ -1447,7 +1462,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="29.1">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B32" s="17" t="s">
         <v>61</v>
       </c>
@@ -1464,7 +1479,7 @@
       </c>
       <c r="H32" s="19"/>
     </row>
-    <row r="33" spans="1:8" ht="29.1">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B33" s="17" t="s">
         <v>63</v>
       </c>
@@ -1483,7 +1498,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="30">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B34" s="17" t="s">
         <v>64</v>
       </c>
@@ -1500,7 +1515,7 @@
       </c>
       <c r="H34" s="19"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B35" s="17" t="s">
         <v>66</v>
       </c>
@@ -1517,7 +1532,7 @@
       </c>
       <c r="H35" s="19"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B36" s="17" t="s">
         <v>68</v>
       </c>
@@ -1536,7 +1551,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B37" s="17" t="s">
         <v>69</v>
       </c>
@@ -1553,7 +1568,7 @@
       </c>
       <c r="H37" s="19"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B38" s="17" t="s">
         <v>70</v>
       </c>
@@ -1570,7 +1585,7 @@
       </c>
       <c r="H38" s="19"/>
     </row>
-    <row r="39" spans="1:8" ht="29.1">
+    <row r="39" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A39" s="1"/>
       <c r="B39" s="17" t="s">
         <v>72</v>
@@ -1588,7 +1603,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B40" s="17" t="s">
         <v>73</v>
       </c>
@@ -1605,6 +1620,76 @@
       <c r="G40" s="19"/>
       <c r="H40" s="19" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A41" s="1"/>
+      <c r="B41" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A42" s="1"/>
+      <c r="B42" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H42" s="19"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A43" s="1"/>
+      <c r="B43" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="H43" s="19"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A44" s="1"/>
+      <c r="B44" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1614,9 +1699,10 @@
     <hyperlink ref="G30" r:id="rId3" xr:uid="{447F93E0-6DD6-4075-8A58-A4CF6F5B315D}"/>
     <hyperlink ref="G34" r:id="rId4" xr:uid="{A7966A6F-DAFE-40B6-8B59-5C61AF02A947}"/>
     <hyperlink ref="G37" r:id="rId5" xr:uid="{5DF8B77B-C500-4050-BB6C-D0B080A9BF59}"/>
+    <hyperlink ref="G43" r:id="rId6" xr:uid="{D24797F3-544D-471D-80A8-C5BC5FC0CAB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1631,14 +1717,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="1025" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -1646,7 +1732,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1654,7 +1740,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1662,17 +1748,17 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -1692,9 +1778,9 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1025" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>